<commit_message>
rtkconv.sh fixed to include SNR
</commit_message>
<xml_diff>
--- a/Brant_Timesheets/2018_Timesheets_Brant.xlsx
+++ b/Brant_Timesheets/2018_Timesheets_Brant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="13380" tabRatio="837" firstSheet="9" activeTab="9"/>
+    <workbookView xWindow="320" yWindow="340" windowWidth="25040" windowHeight="13380" tabRatio="837" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-12-2018" sheetId="77" r:id="rId1"/>
@@ -13547,8 +13547,8 @@
   </sheetPr>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -14075,8 +14075,12 @@
       <c r="D16" s="158">
         <v>0.33333333333333331</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="59"/>
+      <c r="E16" s="59">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="59">
+        <v>0.52083333333333337</v>
+      </c>
       <c r="G16" s="59"/>
       <c r="H16" s="58"/>
       <c r="I16" s="58"/>
@@ -14084,13 +14088,13 @@
       <c r="K16" s="322"/>
       <c r="L16" s="100">
         <f t="shared" si="0"/>
-        <v>-0.33333333333333331</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="M16" s="75"/>
       <c r="N16" s="101"/>
       <c r="O16" s="100">
         <f t="shared" si="1"/>
-        <v>-0.33333333333333331</v>
+        <v>0.16666666666666669</v>
       </c>
       <c r="P16" s="40"/>
       <c r="R16" s="2"/>
@@ -14212,11 +14216,11 @@
       </c>
       <c r="P20" s="155">
         <f>SUM(O14:O20)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q20" s="110">
         <f>P20*24</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R20" s="2"/>
     </row>
@@ -14402,11 +14406,11 @@
       <c r="O27" s="416"/>
       <c r="P27" s="155">
         <f>SUM(O9:O23)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q27" s="110">
         <f>P27*24</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R27" s="2"/>
     </row>

</xml_diff>

<commit_message>
update timesheets and nvsBinrInit.sh
</commit_message>
<xml_diff>
--- a/Brant_Timesheets/2018_Timesheets_Brant.xlsx
+++ b/Brant_Timesheets/2018_Timesheets_Brant.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="540" yWindow="160" windowWidth="25040" windowHeight="13380" tabRatio="837" firstSheet="9" activeTab="10"/>
+    <workbookView xWindow="540" yWindow="160" windowWidth="25040" windowHeight="13380" tabRatio="837" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="1-12-2018" sheetId="77" r:id="rId1"/>
@@ -13547,7 +13547,7 @@
   </sheetPr>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -14894,8 +14894,8 @@
   </sheetPr>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -15494,7 +15494,9 @@
       <c r="C17" s="63">
         <v>43243</v>
       </c>
-      <c r="D17" s="158"/>
+      <c r="D17" s="158">
+        <v>0.4375</v>
+      </c>
       <c r="E17" s="59"/>
       <c r="F17" s="59"/>
       <c r="G17" s="59"/>
@@ -15504,13 +15506,13 @@
       <c r="K17" s="322"/>
       <c r="L17" s="154">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.4375</v>
       </c>
       <c r="M17" s="75"/>
       <c r="N17" s="101"/>
       <c r="O17" s="100">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-0.4375</v>
       </c>
       <c r="P17" s="39"/>
       <c r="R17" s="2"/>
@@ -15603,11 +15605,11 @@
       </c>
       <c r="P20" s="207">
         <f>SUM(O14:O20)</f>
-        <v>0.60416666666666663</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="Q20" s="110">
         <f>P20*24</f>
-        <v>14.5</v>
+        <v>3.9999999999999991</v>
       </c>
       <c r="R20" s="2"/>
     </row>
@@ -15805,11 +15807,11 @@
       <c r="O27" s="416"/>
       <c r="P27" s="155">
         <f>SUM(O10:O25)</f>
-        <v>1.6041666666666665</v>
+        <v>1.1666666666666665</v>
       </c>
       <c r="Q27" s="110">
         <f>P27*24</f>
-        <v>38.5</v>
+        <v>27.999999999999996</v>
       </c>
       <c r="R27" s="2"/>
     </row>

</xml_diff>

<commit_message>
commented out git commands for navFetch
</commit_message>
<xml_diff>
--- a/Brant_Timesheets/2018_Timesheets_Brant.xlsx
+++ b/Brant_Timesheets/2018_Timesheets_Brant.xlsx
@@ -14895,7 +14895,7 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -15497,7 +15497,9 @@
       <c r="D17" s="158">
         <v>0.4375</v>
       </c>
-      <c r="E17" s="59"/>
+      <c r="E17" s="59">
+        <v>0.6875</v>
+      </c>
       <c r="F17" s="59"/>
       <c r="G17" s="59"/>
       <c r="H17" s="58"/>
@@ -15506,13 +15508,13 @@
       <c r="K17" s="322"/>
       <c r="L17" s="154">
         <f t="shared" si="0"/>
-        <v>-0.4375</v>
+        <v>0.25</v>
       </c>
       <c r="M17" s="75"/>
       <c r="N17" s="101"/>
       <c r="O17" s="100">
         <f t="shared" si="1"/>
-        <v>-0.4375</v>
+        <v>0.25</v>
       </c>
       <c r="P17" s="39"/>
       <c r="R17" s="2"/>
@@ -15605,11 +15607,11 @@
       </c>
       <c r="P20" s="207">
         <f>SUM(O14:O20)</f>
-        <v>0.16666666666666663</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="Q20" s="110">
         <f>P20*24</f>
-        <v>3.9999999999999991</v>
+        <v>20.5</v>
       </c>
       <c r="R20" s="2"/>
     </row>
@@ -15807,11 +15809,11 @@
       <c r="O27" s="416"/>
       <c r="P27" s="155">
         <f>SUM(O10:O25)</f>
-        <v>1.1666666666666665</v>
+        <v>1.8541666666666665</v>
       </c>
       <c r="Q27" s="110">
         <f>P27*24</f>
-        <v>27.999999999999996</v>
+        <v>44.5</v>
       </c>
       <c r="R27" s="2"/>
     </row>

</xml_diff>